<commit_message>
Requisito 12-Adicion de Excell de requisitos y informacion de despliegue
</commit_message>
<xml_diff>
--- a/sdi1920-entrega1-914-909.xlsx
+++ b/sdi1920-entrega1-914-909.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Universidad de Oviedo\ENRIQUE ANTONIO DE LA CAL MARIN - SDI\1920\prácticas_propuestas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="11_6F87C70C0EEBBB682A1A7E76B668D25BBE68B5E0" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{224EE973-8D5F-41C5-AC7E-8F558993F90C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FE0B525-CDE7-4C09-B2A2-4662325DC647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8830" yWindow="830" windowWidth="27370" windowHeight="19020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="345" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="72">
   <si>
     <t>Puntuación (Para rellenar por el profesor)</t>
   </si>
@@ -218,6 +220,93 @@
   </si>
   <si>
     <t>Informe</t>
+  </si>
+  <si>
+    <t>Si se pasa una segunda vez de seguido falla porque agrega un usuario que se agrego la vez pasada</t>
+  </si>
+  <si>
+    <t>Una segunda pasada hace que falle este test porque se acepta esta peticion de amistad que se mira en otro punto</t>
+  </si>
+  <si>
+    <t>Una segunda pasada hace que falle porque la vez anterior se acepta la peticion de amistad de la prueba</t>
+  </si>
+  <si>
+    <t>Se comprueban el menú de login,el navegador, mis publicaciones, lista de usuarios, lista de invitaciones</t>
+  </si>
+  <si>
+    <t>Se intenta hacer un registro con un usuario sin nombre, y luego con nombre pero sin el resto de informacion y comprobamos que salta el error especifico para cada falta</t>
+  </si>
+  <si>
+    <t>Se intenta registrar un usuario con contraseña y confirmacion diferentes y comprobamos que salta error concreto, luego probamos con una contraseña demasiado corta y comprobamos que el mensaje de error es el correcto</t>
+  </si>
+  <si>
+    <t>Se intenta registrar un usuario que ya exista en la bbdd y comprobamos que sale el error de email duplicado</t>
+  </si>
+  <si>
+    <t>Nos logeamos como el usuario admin, nos dirigimos a la pantalla de agregar usuario, opción solo accesible para admin, y comprobamos que entró bien</t>
+  </si>
+  <si>
+    <t>Se loggea como usuario normal y comprobamos llendo a la lista de usuarios y se comprueba que no aparece ()</t>
+  </si>
+  <si>
+    <t>Se intenta hacer un login con los campos vacios y comprobamos que sale el mensaje de error de login</t>
+  </si>
+  <si>
+    <t>Se intenta acceder al usuario pedro@gmail.com con una contraseña erronea y comprobamos que salta el mensaje de error de login</t>
+  </si>
+  <si>
+    <t>Se inicia sesion con un usuario cualquiera, se clica la opción de desconexión y se comprueba que redirija a la pantalla de login</t>
+  </si>
+  <si>
+    <t>Se hace un check de la pantalla de identificacion que comprueba todos los componentes que deben aparecer (donde no se deberia ver el boton de Desconexion)</t>
+  </si>
+  <si>
+    <t>Se inicia sesion con un usuario cualquiera, se abre la pantalla de listar usuarios y vemos que estan los usuarios primeros de la pantalla y comprobamos que no aparecen ni el admin ni el usuario logeado</t>
+  </si>
+  <si>
+    <t>Se abre la opcion listar usuarios se hace la busqueda con la barra de busqueda vacia y comprobamos que salen los usuarios pertinentes</t>
+  </si>
+  <si>
+    <t>Se abre la opcion listar usuarios se hace la busqueda con la barra de busqueda con una frase complejo y comprobamos que no sale ningun usuario</t>
+  </si>
+  <si>
+    <t>Se abre la opcion listar usuarios se hace la busqueda con la barra de busqueda con el texto Mar y comprobamos que solo aparecen Maria y Marta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos logeamos como un usuario cuialquiera y le enviamos una invitacion a un usuario, salimos de sesión, nos logeamos como el usuario objetivo y comprobamos que aparece la invitacion recien enviada </t>
+  </si>
+  <si>
+    <t>Nos logeamos como un usuario con una invitacion enviada a un usuario, probamos enviarsela otra vez y comprobamos que sale el mensaje error pertinente</t>
+  </si>
+  <si>
+    <t>Se comprueban el menú de login,el navegador, mis publicaciones, lista de usuarios, lista de invitaciones Nos logeamos como pedro@gmail.com y comprobamos que estan las 3 amistades correspondientes</t>
+  </si>
+  <si>
+    <t>Intentamos acceder al enlace de listar usuarios y comprobamos que nos ha redirigido  a la pantalla de identificación</t>
+  </si>
+  <si>
+    <t>Intentamos acceder al enlace de listar publicaciones  y comprobamos que nos ha redirigido  a la pantalla de identificación</t>
+  </si>
+  <si>
+    <t>Nos logeamos como un usuario admin y comprobamos que podemos acceder al link de listar usuarios, cambiamos de sesion a un usuario estandar, comprobamos que al ir al enlace directamente nos llevan a una pantalla con el error 403</t>
+  </si>
+  <si>
+    <t>Nos logeamos como un usuario, accedemos a la opcion de crear publiaciones  y añadimos una nueva, luego accedemos a la pantalla listar publicaciones  y comprobamos que aparece la nueva</t>
+  </si>
+  <si>
+    <t>Nos logeamos como un usuario, accedemos a la opcion de crear publiaciones  y intentamos crearla con los campos vacios y comprobamos que nos redirigio al listado de publicaciones por crearse la publicacion</t>
+  </si>
+  <si>
+    <t>Nos logeamos como el usuario pedro@gmail.com, nos dirigimos al listado de publicaciones y comprobamos que aparecen las creadas por defecto</t>
+  </si>
+  <si>
+    <t>Nos logeamos como el usuario maral@gmail.com, nos dirigimos al listado de amigos clickamos en en ver detalles de pedro@gmail.com y comprobamos que estan las publicaciones por defecto</t>
+  </si>
+  <si>
+    <t>Nos logeamos como lucasnu@gmai.com y intentamos ir por enlace directo a los detalles de un usuario en concreto del que no es amigo y comprobamos que nos redirige a la lista de usuarios</t>
+  </si>
+  <si>
+    <t>Nos loggeamos como Admin, nos dirigimos a la lista de usuarios y comprobamos que aparecen todos los que tienen que aparecer, el inclusive</t>
   </si>
 </sst>
 </file>
@@ -542,15 +631,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,6 +645,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -589,25 +687,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -894,111 +983,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82:G82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="39.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="7" max="7" width="39.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:8" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A3" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-    </row>
-    <row r="4" spans="1:8" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="39">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="25">
         <f>G31</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-    </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="A5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="39">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:8" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="25">
         <f>G44</f>
         <v>0</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-    </row>
-    <row r="7" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A7" s="37" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A8" s="22">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="28">
         <f>A4-A6</f>
-        <v>0</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-    </row>
-    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:8" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A11" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1022,7 +1111,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1035,7 +1124,7 @@
       </c>
       <c r="D13" s="1">
         <f>COUNTIFS($B$49:$B$96,$A13,$D$49:$D$96,"=OK")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1">
         <f>COUNTIFS($B$49:$B$96,$A13,$D$49:$D$96,"FAIL")</f>
@@ -1043,14 +1132,14 @@
       </c>
       <c r="F13" s="1">
         <f>COUNTIFS($B$49:$B$96,$A13,$D$49:$D$96,"=SIN")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <f>MIN(C13,(D13/B13)*C13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1063,7 +1152,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ref="D14:D30" si="1">COUNTIFS($B$49:$B$96,$A14,$D$49:$D$96,"=OK")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" ref="E14:E30" si="2">COUNTIFS($B$49:$B$96,$A14,$D$49:$D$96,"FAIL")</f>
@@ -1071,14 +1160,14 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ref="F14:F30" si="3">COUNTIFS($B$49:$B$96,$A14,$D$49:$D$96,"=SIN")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" ref="G14:G30" si="4">MIN(C14,(D14/B14)*C14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1091,7 +1180,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="2"/>
@@ -1099,14 +1188,14 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -1119,7 +1208,7 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
@@ -1127,14 +1216,14 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -1147,7 +1236,7 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="2"/>
@@ -1155,14 +1244,14 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -1175,7 +1264,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="2"/>
@@ -1183,14 +1272,14 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -1203,7 +1292,7 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
@@ -1211,14 +1300,14 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>8</v>
       </c>
@@ -1231,7 +1320,7 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
@@ -1239,14 +1328,14 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -1259,7 +1348,7 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
@@ -1267,14 +1356,14 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1287,7 +1376,7 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
@@ -1295,14 +1384,14 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -1315,7 +1404,7 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="2"/>
@@ -1323,37 +1412,37 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
         <v>12</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C24" s="40">
-        <v>1</v>
-      </c>
-      <c r="D24" s="40">
+      <c r="C24" s="18">
+        <v>1</v>
+      </c>
+      <c r="D24" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="18">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1361,7 +1450,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -1374,7 +1463,7 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="2"/>
@@ -1382,14 +1471,14 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -1402,7 +1491,7 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="2"/>
@@ -1410,13 +1499,13 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -1429,7 +1518,7 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="2"/>
@@ -1437,14 +1526,14 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>16</v>
       </c>
@@ -1472,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>17</v>
       </c>
@@ -1485,7 +1574,7 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="2"/>
@@ -1493,14 +1582,14 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>18</v>
       </c>
@@ -1528,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="3">
@@ -1542,150 +1631,150 @@
       </c>
       <c r="G31" s="11">
         <f>SUM(G13:G30)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A32" s="26" t="s">
+    <row r="32" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>1</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>2</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>3</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>4</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>5</v>
       </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>6</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>7</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>8</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>9</v>
       </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>10</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:8" ht="26" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -1702,7 +1791,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1711,7 +1800,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1720,18 +1809,18 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A47" s="29" t="s">
+    <row r="47" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A47" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="31"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="34"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>41</v>
       </c>
@@ -1744,13 +1833,13 @@
       <c r="D48" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -1761,13 +1850,15 @@
         <v>23</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E49" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2</v>
       </c>
@@ -1778,13 +1869,15 @@
         <v>23</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E50" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -1795,13 +1888,15 @@
         <v>23</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" s="18"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E51" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>4</v>
       </c>
@@ -1812,13 +1907,15 @@
         <v>23</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" s="18"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E52" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>5</v>
       </c>
@@ -1829,13 +1926,15 @@
         <v>23</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E53" s="18"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E53" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>6</v>
       </c>
@@ -1846,13 +1945,15 @@
         <v>23</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E54" s="18"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E54" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>7</v>
       </c>
@@ -1863,13 +1964,15 @@
         <v>23</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="18"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E55" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>8</v>
       </c>
@@ -1880,13 +1983,15 @@
         <v>23</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E56" s="18"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E56" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>9</v>
       </c>
@@ -1897,13 +2002,15 @@
         <v>23</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" s="41"/>
+      <c r="G57" s="41"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>10</v>
       </c>
@@ -1914,13 +2021,15 @@
         <v>23</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E58" s="18"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E58" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>11</v>
       </c>
@@ -1931,13 +2040,15 @@
         <v>23</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E59" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>12</v>
       </c>
@@ -1948,13 +2059,15 @@
         <v>23</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E60" s="18"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E60" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>13</v>
       </c>
@@ -1965,13 +2078,15 @@
         <v>23</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" s="18"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E61" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>14</v>
       </c>
@@ -1982,13 +2097,15 @@
         <v>23</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E62" s="18"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E62" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>15</v>
       </c>
@@ -1999,13 +2116,15 @@
         <v>23</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E63" s="18"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E63" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F63" s="41"/>
+      <c r="G63" s="41"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>16</v>
       </c>
@@ -2016,13 +2135,15 @@
         <v>23</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E64" s="18"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E64" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="F64" s="41"/>
+      <c r="G64" s="41"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>17</v>
       </c>
@@ -2033,13 +2154,15 @@
         <v>23</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E65" s="18"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E65" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" s="41"/>
+      <c r="G65" s="41"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>18</v>
       </c>
@@ -2050,13 +2173,15 @@
         <v>23</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E66" s="18"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E66" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" s="41"/>
+      <c r="G66" s="41"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>19</v>
       </c>
@@ -2067,13 +2192,15 @@
         <v>23</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E67" s="18"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E67" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>20</v>
       </c>
@@ -2084,13 +2211,15 @@
         <v>23</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" s="18"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E68" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F68" s="41"/>
+      <c r="G68" s="41"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>21</v>
       </c>
@@ -2101,13 +2230,15 @@
         <v>23</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E69" s="18"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="F69" s="41"/>
+      <c r="G69" s="41"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>22</v>
       </c>
@@ -2118,13 +2249,15 @@
         <v>23</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="18"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="19"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E70" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F70" s="41"/>
+      <c r="G70" s="41"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>23</v>
       </c>
@@ -2135,30 +2268,32 @@
         <v>23</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E71" s="18"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="19"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E71" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F71" s="41"/>
+      <c r="G71" s="41"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B72" s="40">
+      <c r="B72" s="18">
         <v>12</v>
       </c>
-      <c r="C72" s="40" t="s">
+      <c r="C72" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D72" s="40" t="s">
+      <c r="D72" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E72" s="42"/>
       <c r="F72" s="43"/>
       <c r="G72" s="43"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>24</v>
       </c>
@@ -2169,13 +2304,15 @@
         <v>25</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E73" s="18"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E73" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F73" s="41"/>
+      <c r="G73" s="41"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>25</v>
       </c>
@@ -2186,13 +2323,15 @@
         <v>25</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E74" s="18"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>26</v>
       </c>
@@ -2203,13 +2342,13 @@
         <v>25</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E75" s="18"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E75" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>27</v>
       </c>
@@ -2220,13 +2359,15 @@
         <v>25</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E76" s="18"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E76" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="F76" s="41"/>
+      <c r="G76" s="41"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>28</v>
       </c>
@@ -2237,13 +2378,15 @@
         <v>25</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E77" s="18"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E77" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F77" s="41"/>
+      <c r="G77" s="41"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>29</v>
       </c>
@@ -2256,11 +2399,11 @@
       <c r="D78" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E78" s="18"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="19"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E78" s="38"/>
+      <c r="F78" s="41"/>
+      <c r="G78" s="41"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>30</v>
       </c>
@@ -2273,11 +2416,11 @@
       <c r="D79" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E79" s="18"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E79" s="38"/>
+      <c r="F79" s="41"/>
+      <c r="G79" s="41"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>31</v>
       </c>
@@ -2288,13 +2431,15 @@
         <v>25</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E80" s="18"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="19"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E80" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F80" s="41"/>
+      <c r="G80" s="41"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>32</v>
       </c>
@@ -2307,11 +2452,11 @@
       <c r="D81" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E81" s="18"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="19"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E81" s="38"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="41"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>33</v>
       </c>
@@ -2324,11 +2469,11 @@
       <c r="D82" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="18"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E82" s="38"/>
+      <c r="F82" s="41"/>
+      <c r="G82" s="41"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>34</v>
       </c>
@@ -2341,11 +2486,11 @@
       <c r="D83" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="18"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E83" s="38"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="41"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>35</v>
       </c>
@@ -2356,11 +2501,11 @@
       <c r="D84" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E84" s="18"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="19"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E84" s="38"/>
+      <c r="F84" s="41"/>
+      <c r="G84" s="41"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>36</v>
       </c>
@@ -2371,11 +2516,11 @@
       <c r="D85" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E85" s="18"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="19"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E85" s="38"/>
+      <c r="F85" s="41"/>
+      <c r="G85" s="41"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>37</v>
       </c>
@@ -2386,11 +2531,11 @@
       <c r="D86" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E86" s="18"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="19"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E86" s="38"/>
+      <c r="F86" s="41"/>
+      <c r="G86" s="41"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>38</v>
       </c>
@@ -2401,11 +2546,11 @@
       <c r="D87" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E87" s="18"/>
-      <c r="F87" s="19"/>
-      <c r="G87" s="19"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E87" s="38"/>
+      <c r="F87" s="41"/>
+      <c r="G87" s="41"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>39</v>
       </c>
@@ -2416,11 +2561,11 @@
       <c r="D88" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E88" s="18"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="19"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E88" s="38"/>
+      <c r="F88" s="41"/>
+      <c r="G88" s="41"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>40</v>
       </c>
@@ -2431,11 +2576,11 @@
       <c r="D89" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E89" s="18"/>
-      <c r="F89" s="19"/>
-      <c r="G89" s="19"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E89" s="38"/>
+      <c r="F89" s="41"/>
+      <c r="G89" s="41"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>41</v>
       </c>
@@ -2446,11 +2591,11 @@
       <c r="D90" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E90" s="18"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="19"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E90" s="38"/>
+      <c r="F90" s="41"/>
+      <c r="G90" s="41"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>42</v>
       </c>
@@ -2461,11 +2606,11 @@
       <c r="D91" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E91" s="18"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="19"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E91" s="38"/>
+      <c r="F91" s="41"/>
+      <c r="G91" s="41"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>43</v>
       </c>
@@ -2476,11 +2621,11 @@
       <c r="D92" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E92" s="18"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="19"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E92" s="38"/>
+      <c r="F92" s="41"/>
+      <c r="G92" s="41"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44</v>
       </c>
@@ -2491,11 +2636,11 @@
       <c r="D93" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E93" s="18"/>
-      <c r="F93" s="19"/>
-      <c r="G93" s="19"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E93" s="38"/>
+      <c r="F93" s="41"/>
+      <c r="G93" s="41"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45</v>
       </c>
@@ -2506,11 +2651,11 @@
       <c r="D94" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E94" s="18"/>
-      <c r="F94" s="19"/>
-      <c r="G94" s="19"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E94" s="38"/>
+      <c r="F94" s="41"/>
+      <c r="G94" s="41"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>46</v>
       </c>
@@ -2521,11 +2666,11 @@
       <c r="D95" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E95" s="18"/>
-      <c r="F95" s="19"/>
-      <c r="G95" s="19"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E95" s="38"/>
+      <c r="F95" s="41"/>
+      <c r="G95" s="41"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>47</v>
       </c>
@@ -2536,18 +2681,59 @@
       <c r="D96" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E96" s="18"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="19"/>
+      <c r="E96" s="38"/>
+      <c r="F96" s="41"/>
+      <c r="G96" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="70">
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
+  <mergeCells count="69">
+    <mergeCell ref="E96:G96"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="E93:G93"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A11:G11"/>
@@ -2564,54 +2750,12 @@
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="B43:F43"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="E96:G96"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="E88:G88"/>
-    <mergeCell ref="E89:G89"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="E93:G93"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2640,33 +2784,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -2674,7 +2818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
@@ -2682,7 +2826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
@@ -2690,7 +2834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
@@ -2698,8 +2842,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
@@ -2707,7 +2851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2715,7 +2859,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>35</v>
       </c>
@@ -2723,7 +2867,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>37</v>
       </c>

</xml_diff>